<commit_message>
Changed syntax and processing to allow for multi-dimensional key names
</commit_message>
<xml_diff>
--- a/test/templates/t1.xlsx
+++ b/test/templates/t1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="15990" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,15 +30,6 @@
     <t>Plan table</t>
   </si>
   <si>
-    <t>${table:planData.name}</t>
-  </si>
-  <si>
-    <t>${table:planData.role}</t>
-  </si>
-  <si>
-    <t>${table:planData.days}</t>
-  </si>
-  <si>
     <t>${dates}</t>
   </si>
   <si>
@@ -46,16 +37,25 @@
   </si>
   <si>
     <t>Extracted on ${extractDate}</t>
+  </si>
+  <si>
+    <t>${table:planData:name}</t>
+  </si>
+  <si>
+    <t>${table:planData:role}</t>
+  </si>
+  <si>
+    <t>${table:planData:days}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -202,21 +202,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="4" builtinId="4"/>
@@ -551,39 +551,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:D7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="20" thickBot="1">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:4" ht="20.25" thickBot="1">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="2:4" ht="14" thickTop="1"/>
+    <row r="3" spans="2:4" ht="13.5" thickTop="1"/>
     <row r="4" spans="2:4">
-      <c r="B4" s="7" t="s">
-        <v>8</v>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="8"/>
+      <c r="B5" s="5"/>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="1" t="s">
@@ -593,18 +591,18 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>5</v>
+      <c r="B7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>